<commit_message>
wrote the jsp file and the servlet file
</commit_message>
<xml_diff>
--- a/documents/DB_Definition.xlsx
+++ b/documents/DB_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bbs11\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E10F760-89E5-401A-8022-FF5473D33848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B260C22-DE18-4C0C-A751-1C17B2A4D685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{B0F827ED-2CE3-7C48-886C-2585E81B6661}"/>
+    <workbookView minimized="1" xWindow="3140" yWindow="2810" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{B0F827ED-2CE3-7C48-886C-2585E81B6661}"/>
   </bookViews>
   <sheets>
     <sheet name="DB定義書" sheetId="1" r:id="rId1"/>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1A30F9-296F-1F4C-A124-61C5E9B81C48}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="20" x14ac:dyDescent="0.6"/>
@@ -1283,8 +1283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D59648-6F36-FA48-AB43-167306A08336}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="20" x14ac:dyDescent="0.6"/>
@@ -1378,6 +1378,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1385,7 +1386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2786C910-DBE5-3D48-94A8-089EA7E4D828}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -1723,7 +1724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA691B61-B856-E245-9244-6BE6218F09F7}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>